<commit_message>
excel update 2-3 file
</commit_message>
<xml_diff>
--- a/URS_Certifications-2.xlsx
+++ b/URS_Certifications-2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\сайт\сайт2\Сайт на практику\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A86E95-495C-4608-9D63-BE8FB8BEEB58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4327AB6A-0B69-4245-80E3-111ED6E89F7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2633,7 +2633,7 @@
   <dimension ref="A1:G1345"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="G66" sqref="G66"/>
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>